<commit_message>
Einkauf getränke neu berechnet. Schüwo mit TabBar
</commit_message>
<xml_diff>
--- a/Input/Einkauf Kiosk  01.11.23.xlsx
+++ b/Input/Einkauf Kiosk  01.11.23.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub 2024\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R Packages\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17AD3F6-CFDF-4F47-83CF-BBE350BF70D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C012FB03-91A7-4206-BE20-241B004A17C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{B11F654B-1788-4E85-B872-7BAC8A50C723}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B11F654B-1788-4E85-B872-7BAC8A50C723}"/>
   </bookViews>
   <sheets>
     <sheet name="KinoKiosk Angebot 2023" sheetId="1" r:id="rId1"/>
@@ -1134,22 +1134,22 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="33.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="1" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="9" width="13" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="15" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="15" customFormat="1" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>21</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0.3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G12" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1487,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>31</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>32</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>49</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>75</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>15</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>53</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>27</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>28</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34" s="8"/>
@@ -2125,14 +2125,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>45</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Tschugger und DSDMT -11.-13.10.24 Filmvorführungen
</commit_message>
<xml_diff>
--- a/Input/Einkauf Kiosk  01.11.23.xlsx
+++ b/Input/Einkauf Kiosk  01.11.23.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kinoklub\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E0D65D-E180-4DE6-9C21-293124DA9F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F35BE4-71A9-41E7-AA86-EB6B765F924D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{B11F654B-1788-4E85-B872-7BAC8A50C723}"/>
+    <workbookView xWindow="5460" yWindow="5568" windowWidth="15684" windowHeight="11832" xr2:uid="{B11F654B-1788-4E85-B872-7BAC8A50C723}"/>
   </bookViews>
   <sheets>
     <sheet name="KinoKiosk Angebot 2023" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="95">
   <si>
     <t>Schüwo</t>
   </si>
@@ -108,21 +108,6 @@
     <t>Gewinn</t>
   </si>
   <si>
-    <t>Glalcé Schoggi</t>
-  </si>
-  <si>
-    <t>Glalcé Mocca</t>
-  </si>
-  <si>
-    <t>Glalcé Mango</t>
-  </si>
-  <si>
-    <t>Glalcé Erdbeere</t>
-  </si>
-  <si>
-    <t>Glalcé Caramel</t>
-  </si>
-  <si>
     <t>Gazosa Orange</t>
   </si>
   <si>
@@ -289,6 +274,54 @@
   </si>
   <si>
     <t>Anzahl Bestellung Feb 2024</t>
+  </si>
+  <si>
+    <t>Glacé Caramel</t>
+  </si>
+  <si>
+    <t>Glacé Erdbeere</t>
+  </si>
+  <si>
+    <t>Glacé Mango</t>
+  </si>
+  <si>
+    <t>Glacé Mocca</t>
+  </si>
+  <si>
+    <t>Glacé Schoggi</t>
+  </si>
+  <si>
+    <t>Glacé Schokolade</t>
+  </si>
+  <si>
+    <t>Schokolade</t>
+  </si>
+  <si>
+    <t>Glacé weisser Kaffee</t>
+  </si>
+  <si>
+    <t>Glacé Pistache</t>
+  </si>
+  <si>
+    <t>Pistache</t>
+  </si>
+  <si>
+    <t>Sorbet Zitronen-Rosmarin</t>
+  </si>
+  <si>
+    <t>Sorbet Himbeer</t>
+  </si>
+  <si>
+    <t>Zitronen-Rosmarinsorbet</t>
+  </si>
+  <si>
+    <t>Himbeersorbet</t>
+  </si>
+  <si>
+    <t>Crazy for Gelato</t>
+  </si>
+  <si>
+    <t>Weisser Kaffee</t>
   </si>
 </sst>
 </file>
@@ -329,7 +362,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -393,11 +426,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -422,6 +468,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,8 +846,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{920C96DA-BD94-48CE-B13B-7B1D665A1F1C}" name="Table1" displayName="Table1" ref="A1:I33" headerRowDxfId="19" totalsRowDxfId="18">
-  <autoFilter ref="A1:I33" xr:uid="{920C96DA-BD94-48CE-B13B-7B1D665A1F1C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{920C96DA-BD94-48CE-B13B-7B1D665A1F1C}" name="Table1" displayName="Table1" ref="A1:I38" headerRowDxfId="19" totalsRowDxfId="18">
+  <autoFilter ref="A1:I38" xr:uid="{920C96DA-BD94-48CE-B13B-7B1D665A1F1C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E8635A23-EB85-4436-9D20-6BDBA55F1730}" name="Artikel" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="16"/>
     <tableColumn id="4" xr3:uid="{3577DE02-0CD1-4A73-82D1-7EE95A59F5D7}" name="Artikelname Kassensystem" dataDxfId="15" totalsRowDxfId="14"/>
@@ -1128,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A677428D-B810-4F63-BFBD-79DB0D9DB708}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1151,16 +1199,16 @@
         <v>20</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>21</v>
@@ -1169,24 +1217,24 @@
         <v>22</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E2" s="5">
         <v>1.38</v>
@@ -1206,16 +1254,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C3" s="5">
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E3" s="5">
         <v>1.65</v>
@@ -1292,7 +1340,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C6" s="5">
         <v>4</v>
@@ -1302,7 +1350,7 @@
         <v>0.15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G6" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1316,10 +1364,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5">
         <v>4</v>
@@ -1329,7 +1377,7 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G7" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1352,7 +1400,7 @@
         <v>4.5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E8" s="5">
         <v>1.55</v>
@@ -1381,7 +1429,7 @@
         <v>4.5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E9" s="5">
         <v>1.55</v>
@@ -1410,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E10" s="5">
         <v>0.97</v>
@@ -1439,7 +1487,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E11" s="5">
         <v>0.97</v>
@@ -1472,7 +1520,7 @@
         <v>0.3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G12" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1489,13 +1537,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C13" s="5">
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E13" s="5">
         <v>1.1499999999999999</v>
@@ -1518,13 +1566,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C14" s="5">
         <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E14" s="5">
         <v>1.1499999999999999</v>
@@ -1544,16 +1592,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C15" s="5">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E15" s="5">
         <v>1.44</v>
@@ -1582,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E16" s="5">
         <v>1.1200000000000001</v>
@@ -1602,16 +1650,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C17" s="5">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E17" s="5">
         <v>1.44</v>
@@ -1631,16 +1679,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C18" s="5">
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E18" s="5">
         <v>1.44</v>
@@ -1660,16 +1708,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C19" s="6">
         <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E19" s="6">
         <v>1.03</v>
@@ -1698,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E20" s="7">
         <v>1.95</v>
@@ -1718,16 +1766,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C21" s="5">
         <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E21" s="5">
         <v>2.2000000000000002</v>
@@ -1747,22 +1795,22 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5">
         <v>5</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E22" s="5">
         <v>0.4</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G22" s="5">
         <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
@@ -1785,7 +1833,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E23" s="7">
         <v>4.17</v>
@@ -1814,7 +1862,7 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E24" s="5">
         <v>1.06</v>
@@ -1843,7 +1891,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E25" s="5">
         <v>1.06</v>
@@ -1872,7 +1920,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E26" s="5">
         <v>1.06</v>
@@ -1901,7 +1949,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E27" s="5">
         <v>1.06</v>
@@ -1921,16 +1969,16 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C28" s="6">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E28" s="6">
         <v>0.99</v>
@@ -1950,16 +1998,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C29" s="5">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E29" s="5">
         <v>2.2999999999999998</v>
@@ -1979,16 +2027,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C30" s="5">
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E30" s="5">
         <v>2.2999999999999998</v>
@@ -2008,16 +2056,16 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>25</v>
+        <v>81</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C31" s="5">
         <v>4</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E31" s="5">
         <v>2.2999999999999998</v>
@@ -2037,16 +2085,16 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C32" s="5">
         <v>4</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E32" s="5">
         <v>2.2999999999999998</v>
@@ -2066,16 +2114,16 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E33" s="5">
         <v>2.2999999999999998</v>
@@ -2094,15 +2142,149 @@
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34" s="8"/>
-      <c r="D34"/>
-      <c r="E34" s="8"/>
-      <c r="F34"/>
-      <c r="G34" s="8"/>
-      <c r="H34"/>
-      <c r="I34" s="8"/>
+      <c r="A34" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="5">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="17">
+        <v>3</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="17">
+        <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>1</v>
+      </c>
+      <c r="H34" s="16"/>
+      <c r="I34" s="17">
+        <f>Table1[[#This Row],[Anzahl Bestellung Feb 2024]]*Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="5">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="17">
+        <v>3</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G35" s="17">
+        <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="16"/>
+      <c r="I35" s="17">
+        <f>Table1[[#This Row],[Anzahl Bestellung Feb 2024]]*Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="5">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="17">
+        <v>3</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G36" s="17">
+        <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>1</v>
+      </c>
+      <c r="H36" s="16"/>
+      <c r="I36" s="17">
+        <f>Table1[[#This Row],[Anzahl Bestellung Feb 2024]]*Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="5">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="17">
+        <v>3</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="17">
+        <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>1</v>
+      </c>
+      <c r="H37" s="16"/>
+      <c r="I37" s="17">
+        <f>Table1[[#This Row],[Anzahl Bestellung Feb 2024]]*Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="5">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="17">
+        <v>3</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="17">
+        <f>Table1[[#This Row],[Verkaufs-preis]]-Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>1</v>
+      </c>
+      <c r="H38" s="16"/>
+      <c r="I38" s="17">
+        <f>Table1[[#This Row],[Anzahl Bestellung Feb 2024]]*Table1[[#This Row],[Einkaufs- preis]]</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2131,18 +2313,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -2153,7 +2335,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -2161,7 +2343,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -2169,7 +2351,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5">
         <v>6</v>
@@ -2177,7 +2359,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -2185,7 +2367,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -2193,7 +2375,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -2201,7 +2383,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -2209,7 +2391,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -2217,7 +2399,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -2225,7 +2407,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -2233,7 +2415,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B13">
         <v>12</v>

</xml_diff>